<commit_message>
Added json with results of queries and updates excels
</commit_message>
<xml_diff>
--- a/solr/solrMetrics/q1/q1Metrics.xlsx
+++ b/solr/solrMetrics/q1/q1Metrics.xlsx
@@ -445,28 +445,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.833333333333333</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.714285714285714</c:v>
+                  <c:v>0.285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.625</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.555555555555556</c:v>
+                  <c:v>0.222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -575,31 +575,31 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.6</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.428571428571429</c:v>
+                  <c:v>0.571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.375</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.4</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -714,25 +714,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.857142857142857</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>0.666666666666667</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.571428571428571</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.555555555555556</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,11 +747,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6234099"/>
-        <c:axId val="17948618"/>
+        <c:axId val="23934566"/>
+        <c:axId val="23910874"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6234099"/>
+        <c:axId val="23934566"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +812,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17948618"/>
+        <c:crossAx val="23910874"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -820,7 +820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17948618"/>
+        <c:axId val="23910874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +891,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6234099"/>
+        <c:crossAx val="23934566"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1113,16 +1113,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.833333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.833333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.833333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.833333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,28 +1240,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.6</c:v>
+                  <c:v>0.571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.444444444444444</c:v>
+                  <c:v>0.571428571428571</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.444444444444444</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.444444444444444</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,16 +1391,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.555555555555556</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.555555555555556</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1415,11 +1415,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="42409964"/>
-        <c:axId val="60625298"/>
+        <c:axId val="87396158"/>
+        <c:axId val="67425951"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42409964"/>
+        <c:axId val="87396158"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,7 +1488,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60625298"/>
+        <c:crossAx val="67425951"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1496,7 +1496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60625298"/>
+        <c:axId val="67425951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,7 +1539,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42409964"/>
+        <c:crossAx val="87396158"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1741,11 +1741,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="7838831"/>
-        <c:axId val="910178"/>
+        <c:axId val="70520917"/>
+        <c:axId val="24891946"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="7838831"/>
+        <c:axId val="70520917"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1814,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="910178"/>
+        <c:crossAx val="24891946"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1822,7 +1822,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="910178"/>
+        <c:axId val="24891946"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,7 +1901,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7838831"/>
+        <c:crossAx val="70520917"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2135,11 +2135,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="74084607"/>
-        <c:axId val="52878534"/>
+        <c:axId val="65683557"/>
+        <c:axId val="59970157"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74084607"/>
+        <c:axId val="65683557"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2208,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52878534"/>
+        <c:crossAx val="59970157"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2216,7 +2216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52878534"/>
+        <c:axId val="59970157"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,7 +2295,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74084607"/>
+        <c:crossAx val="65683557"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2359,9 +2359,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>632880</xdr:colOff>
+      <xdr:colOff>632520</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2370,7 +2370,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1440000" y="4924440"/>
-        <a:ext cx="5108400" cy="3152160"/>
+        <a:ext cx="5108040" cy="3151800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2389,9 +2389,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>428040</xdr:colOff>
+      <xdr:colOff>427680</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2400,7 +2400,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7053480" y="4857480"/>
-        <a:ext cx="5111280" cy="3152160"/>
+        <a:ext cx="5116680" cy="3151800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2424,9 +2424,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>793080</xdr:colOff>
+      <xdr:colOff>792720</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2434,8 +2434,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4647240" y="2724120"/>
-        <a:ext cx="4357080" cy="2666160"/>
+        <a:off x="4648320" y="2724120"/>
+        <a:ext cx="4361760" cy="2665800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2454,9 +2454,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
+      <xdr:colOff>801360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2465,7 +2465,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="200160" y="2724120"/>
-        <a:ext cx="4352040" cy="2666160"/>
+        <a:ext cx="4351680" cy="2665800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2485,11 +2485,11 @@
   </sheetPr>
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="9.51"/>
@@ -2588,15 +2588,15 @@
       </c>
       <c r="J4" s="5" t="n">
         <f aca="false">SUMIF(B$4:B4,"=1")/SUMIF(B$4:B$23,"=1")</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="K4" s="5" t="n">
         <f aca="false">SUMIF(C$4:C4,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="L4" s="5" t="n">
         <f aca="false">SUMIF(D$4:D4,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.2</v>
+        <v>0.142857142857143</v>
       </c>
       <c r="N4" s="6" t="n">
         <v>0</v>
@@ -2622,7 +2622,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>1</v>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="G5" s="5" t="n">
         <f aca="false">SUM(C$4:C5)/A5</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H5" s="5" t="n">
         <f aca="false">SUM(D$4:D5)/A5</f>
@@ -2641,15 +2641,15 @@
       </c>
       <c r="J5" s="5" t="n">
         <f aca="false">SUMIF(B$4:B5,"=1")/SUMIF(B$4:B$23,"=1")</f>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="K5" s="5" t="n">
         <f aca="false">SUMIF(C$4:C5,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="L5" s="5" t="n">
         <f aca="false">SUMIF(D$4:D5,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.4</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="N5" s="6" t="n">
         <v>0.1</v>
@@ -2671,9 +2671,7 @@
       <c r="A6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="B6" s="4"/>
       <c r="C6" s="4" t="n">
         <v>0</v>
       </c>
@@ -2682,11 +2680,11 @@
       </c>
       <c r="F6" s="5" t="n">
         <f aca="false">SUM(B$4:B6)/A6</f>
-        <v>1</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="G6" s="5" t="n">
         <f aca="false">SUM(C$4:C6)/A6</f>
-        <v>0.666666666666667</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="H6" s="5" t="n">
         <f aca="false">SUM(D$4:D6)/A6</f>
@@ -2694,15 +2692,15 @@
       </c>
       <c r="J6" s="5" t="n">
         <f aca="false">SUMIF(B$4:B6,"=1")/SUMIF(B$4:B$23,"=1")</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="K6" s="5" t="n">
         <f aca="false">SUMIF(C$4:C6,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="L6" s="5" t="n">
         <f aca="false">SUMIF(D$4:D6,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.6</v>
+        <v>0.428571428571429</v>
       </c>
       <c r="N6" s="6" t="n">
         <v>0.2</v>
@@ -2724,18 +2722,16 @@
       <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="5" t="n">
         <f aca="false">SUM(B$4:B7)/A7</f>
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="G7" s="5" t="n">
         <f aca="false">SUM(C$4:C7)/A7</f>
@@ -2743,19 +2739,19 @@
       </c>
       <c r="H7" s="5" t="n">
         <f aca="false">SUM(D$4:D7)/A7</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J7" s="5" t="n">
         <f aca="false">SUMIF(B$4:B7,"=1")/SUMIF(B$4:B$23,"=1")</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="K7" s="5" t="n">
         <f aca="false">SUMIF(C$4:C7,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L7" s="5" t="n">
         <f aca="false">SUMIF(D$4:D7,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.6</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="N7" s="6" t="n">
         <v>0.3</v>
@@ -2766,7 +2762,7 @@
       </c>
       <c r="P7" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N7)</f>
-        <v>1</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="Q7" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N7)</f>
@@ -2777,38 +2773,36 @@
       <c r="A8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="5" t="n">
         <f aca="false">SUM(B$4:B8)/A8</f>
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="G8" s="5" t="n">
         <f aca="false">SUM(C$4:C8)/A8</f>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="H8" s="5" t="n">
         <f aca="false">SUM(D$4:D8)/A8</f>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J8" s="5" t="n">
         <f aca="false">SUMIF(B$4:B8,"=1")/SUMIF(B$4:B$23,"=1")</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K8" s="5" t="n">
         <f aca="false">SUMIF(C$4:C8,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="L8" s="5" t="n">
         <f aca="false">SUMIF(D$4:D8,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.6</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="N8" s="6" t="n">
         <v>0.4</v>
@@ -2819,7 +2813,7 @@
       </c>
       <c r="P8" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N8)</f>
-        <v>1</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="Q8" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N8)</f>
@@ -2830,18 +2824,16 @@
       <c r="A9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>1</v>
-      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="5" t="n">
         <f aca="false">SUM(B$4:B9)/A9</f>
-        <v>0.833333333333333</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="G9" s="5" t="n">
         <f aca="false">SUM(C$4:C9)/A9</f>
@@ -2849,7 +2841,7 @@
       </c>
       <c r="H9" s="5" t="n">
         <f aca="false">SUM(D$4:D9)/A9</f>
-        <v>0.666666666666667</v>
+        <v>1</v>
       </c>
       <c r="J9" s="5" t="n">
         <f aca="false">SUMIF(B$4:B9,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -2857,11 +2849,11 @@
       </c>
       <c r="K9" s="5" t="n">
         <f aca="false">SUMIF(C$4:C9,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="L9" s="5" t="n">
         <f aca="false">SUMIF(D$4:D9,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.8</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="N9" s="6" t="n">
         <v>0.5</v>
@@ -2872,7 +2864,7 @@
       </c>
       <c r="P9" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N9)</f>
-        <v>1</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="Q9" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N9)</f>
@@ -2883,26 +2875,24 @@
       <c r="A10" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B10" s="4"/>
       <c r="C10" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="4" t="n">
         <v>0</v>
       </c>
       <c r="F10" s="5" t="n">
         <f aca="false">SUM(B$4:B10)/A10</f>
-        <v>0.714285714285714</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="G10" s="5" t="n">
         <f aca="false">SUM(C$4:C10)/A10</f>
-        <v>0.428571428571429</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="H10" s="5" t="n">
         <f aca="false">SUM(D$4:D10)/A10</f>
-        <v>0.571428571428571</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="J10" s="5" t="n">
         <f aca="false">SUMIF(B$4:B10,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -2910,11 +2900,11 @@
       </c>
       <c r="K10" s="5" t="n">
         <f aca="false">SUMIF(C$4:C10,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="L10" s="5" t="n">
         <f aca="false">SUMIF(D$4:D10,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.8</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="N10" s="6" t="n">
         <v>0.6</v>
@@ -2925,7 +2915,7 @@
       </c>
       <c r="P10" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N10)</f>
-        <v>0.6</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="Q10" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N10)</f>
@@ -2936,9 +2926,7 @@
       <c r="A11" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="4" t="n">
         <v>0</v>
       </c>
@@ -2947,15 +2935,15 @@
       </c>
       <c r="F11" s="5" t="n">
         <f aca="false">SUM(B$4:B11)/A11</f>
-        <v>0.625</v>
+        <v>0.25</v>
       </c>
       <c r="G11" s="5" t="n">
         <f aca="false">SUM(C$4:C11)/A11</f>
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="5" t="n">
         <f aca="false">SUM(D$4:D11)/A11</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J11" s="5" t="n">
         <f aca="false">SUMIF(B$4:B11,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -2963,44 +2951,42 @@
       </c>
       <c r="K11" s="5" t="n">
         <f aca="false">SUMIF(C$4:C11,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="L11" s="5" t="n">
         <f aca="false">SUMIF(D$4:D11,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>0.8</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="N11" s="6" t="n">
         <v>0.7</v>
       </c>
       <c r="O11" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N11)</f>
-        <v>0.833333333333333</v>
+        <v>1</v>
       </c>
       <c r="P11" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N11)</f>
-        <v>0.6</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="Q11" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N11)</f>
-        <v>0.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C12" s="4" t="n">
-        <v>1</v>
-      </c>
       <c r="D12" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="5" t="n">
         <f aca="false">SUM(B$4:B12)/A12</f>
-        <v>0.555555555555556</v>
+        <v>0.222222222222222</v>
       </c>
       <c r="G12" s="5" t="n">
         <f aca="false">SUM(C$4:C12)/A12</f>
@@ -3008,7 +2994,7 @@
       </c>
       <c r="H12" s="5" t="n">
         <f aca="false">SUM(D$4:D12)/A12</f>
-        <v>0.555555555555556</v>
+        <v>0.666666666666667</v>
       </c>
       <c r="J12" s="5" t="n">
         <f aca="false">SUMIF(B$4:B12,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -3016,52 +3002,50 @@
       </c>
       <c r="K12" s="5" t="n">
         <f aca="false">SUMIF(C$4:C12,"=1")/SUMIF(C$4:C$23,"=1")</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="L12" s="5" t="n">
         <f aca="false">SUMIF(D$4:D12,"=1")/SUMIF(D$4:D$23,"=1")</f>
-        <v>1</v>
+        <v>0.857142857142857</v>
       </c>
       <c r="N12" s="6" t="n">
         <v>0.8</v>
       </c>
       <c r="O12" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N12)</f>
-        <v>0.833333333333333</v>
+        <v>1</v>
       </c>
       <c r="P12" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N12)</f>
-        <v>0.444444444444444</v>
+        <v>0.571428571428571</v>
       </c>
       <c r="Q12" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N12)</f>
-        <v>0.666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="4" t="n">
-        <v>0</v>
-      </c>
+      <c r="B13" s="4"/>
       <c r="C13" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="5" t="n">
         <f aca="false">SUM(B$4:B13)/A13</f>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="G13" s="5" t="n">
         <f aca="false">SUM(C$4:C13)/A13</f>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H13" s="5" t="n">
         <f aca="false">SUM(D$4:D13)/A13</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J13" s="5" t="n">
         <f aca="false">SUMIF(B$4:B13,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -3080,15 +3064,15 @@
       </c>
       <c r="O13" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N13)</f>
-        <v>0.833333333333333</v>
+        <v>1</v>
       </c>
       <c r="P13" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N13)</f>
-        <v>0.444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="Q13" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N13)</f>
-        <v>0.555555555555556</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,15 +3091,15 @@
       </c>
       <c r="O14" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N14)</f>
-        <v>0.833333333333333</v>
+        <v>1</v>
       </c>
       <c r="P14" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N14)</f>
-        <v>0.444444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="Q14" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N14)</f>
-        <v>0.555555555555556</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,15 +3216,15 @@
       </c>
       <c r="F25" s="5" t="n">
         <f aca="false">AVERAGE(F4:F13)</f>
-        <v>0.77781746031746</v>
+        <v>0.485793650793651</v>
       </c>
       <c r="G25" s="5" t="n">
         <f aca="false">AVERAGE(G4:G13)</f>
-        <v>0.591468253968254</v>
+        <v>0.524920634920635</v>
       </c>
       <c r="H25" s="5" t="n">
         <f aca="false">AVERAGE(H4:H13)</f>
-        <v>0.714365079365079</v>
+        <v>0.897380952380952</v>
       </c>
     </row>
   </sheetData>
@@ -3271,7 +3255,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.75"/>

</xml_diff>